<commit_message>
Alterações na tela de conciliação bancaria
</commit_message>
<xml_diff>
--- a/cypress/downloads/DashboardPagamentos.xlsx
+++ b/cypress/downloads/DashboardPagamentos.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Descrição</t>
   </si>
@@ -32,16 +32,7 @@
     <t>Total(%)</t>
   </si>
   <si>
-    <t>Empresa Modelo</t>
-  </si>
-  <si>
-    <t>148.622,77</t>
-  </si>
-  <si>
-    <t>-373,65</t>
-  </si>
-  <si>
-    <t>148.249,12</t>
+    <t>0,00</t>
   </si>
 </sst>
 </file>
@@ -158,38 +149,21 @@
       </c>
     </row>
     <row r="2" spans="1:5" outlineLevel="0" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s"/>
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="n">
-        <v>148622.773203</v>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
       </c>
-      <c r="C2" s="4" t="n">
-        <v>-373.65</v>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
       </c>
-      <c r="D2" s="4" t="n">
-        <v>148249.123203</v>
-      </c>
-      <c r="E2" s="5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" outlineLevel="0" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s"/>
-      <c r="B3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1" t="s"/>
+      <c r="E2" s="1" t="s"/>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError sqref="A1:E3" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:E2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Novos parametros no JenkinsFile
</commit_message>
<xml_diff>
--- a/cypress/downloads/DashboardPagamentos.xlsx
+++ b/cypress/downloads/DashboardPagamentos.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Descrição</t>
   </si>
@@ -32,7 +32,16 @@
     <t>Total(%)</t>
   </si>
   <si>
-    <t>0,00</t>
+    <t>Empresa Modelo</t>
+  </si>
+  <si>
+    <t>148.622,77</t>
+  </si>
+  <si>
+    <t>-373,65</t>
+  </si>
+  <si>
+    <t>148.249,12</t>
   </si>
 </sst>
 </file>
@@ -149,21 +158,38 @@
       </c>
     </row>
     <row r="2" spans="1:5" outlineLevel="0" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s"/>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
+      <c r="B2" s="4" t="n">
+        <v>148622.773203</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>5</v>
+      <c r="C2" s="4" t="n">
+        <v>-373.65</v>
       </c>
-      <c r="E2" s="1" t="s"/>
+      <c r="D2" s="4" t="n">
+        <v>148249.123203</v>
+      </c>
+      <c r="E2" s="5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" outlineLevel="0" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s"/>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s"/>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError sqref="A1:E2" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:E3" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
corrigindo dashboard e conciliacao bancaria 2
</commit_message>
<xml_diff>
--- a/cypress/downloads/DashboardPagamentos.xlsx
+++ b/cypress/downloads/DashboardPagamentos.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Descrição</t>
   </si>
@@ -32,7 +32,16 @@
     <t>Total(%)</t>
   </si>
   <si>
-    <t>0,00</t>
+    <t>Empresa Modelo</t>
+  </si>
+  <si>
+    <t>148.622,77</t>
+  </si>
+  <si>
+    <t>-373,65</t>
+  </si>
+  <si>
+    <t>148.249,12</t>
   </si>
 </sst>
 </file>
@@ -125,10 +134,10 @@
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" x14ac:dyDescent="0.25"/>
   <cols>
     <col width="33.57" min="1" max="1" customWidth="1"/>
-    <col width="20.86" min="2" max="2" customWidth="1"/>
-    <col width="20.86" min="3" max="3" customWidth="1"/>
-    <col width="20.86" min="4" max="4" customWidth="1"/>
-    <col width="20.86" min="5" max="5" customWidth="1"/>
+    <col width="21" min="2" max="2" customWidth="1"/>
+    <col width="21" min="3" max="3" customWidth="1"/>
+    <col width="21" min="4" max="4" customWidth="1"/>
+    <col width="21" min="5" max="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" outlineLevel="0" x14ac:dyDescent="0.25">
@@ -149,21 +158,38 @@
       </c>
     </row>
     <row r="2" spans="1:5" outlineLevel="0" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s"/>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
+      <c r="B2" s="4" t="n">
+        <v>148622.773203</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>5</v>
+      <c r="C2" s="4" t="n">
+        <v>-373.65</v>
       </c>
-      <c r="E2" s="1" t="s"/>
+      <c r="D2" s="4" t="n">
+        <v>148249.123203</v>
+      </c>
+      <c r="E2" s="5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" outlineLevel="0" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s"/>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s"/>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError sqref="A1:E2" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:E3" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>